<commit_message>
Code review points verified
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56382C\Documents\UiPath\P004_SP003_090_NewHireCommunication_WorkdayDispositionApproval_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF56FC8-D7D8-40EA-8E9F-7CA18261FDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51646635-C73C-4E00-935A-ED15CF079060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="124">
   <si>
     <t>Name</t>
   </si>
@@ -152,12 +152,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>HiringManagerTemplatePath</t>
-  </si>
-  <si>
-    <t>WelcomeEmailTemplatePath</t>
-  </si>
-  <si>
     <t>EmailAccount</t>
   </si>
   <si>
@@ -194,12 +188,6 @@
     <t>O365ApplicationSecret</t>
   </si>
   <si>
-    <t>C:\Users\56382C\Documents\Hiring Manager Template.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\56382C\Documents\Welcome Email Template.xlsx</t>
-  </si>
-  <si>
     <t>DEV</t>
   </si>
   <si>
@@ -258,6 +246,178 @@
   </si>
   <si>
     <t>DelayTimeKeys</t>
+  </si>
+  <si>
+    <t>SystemException_EmailSubject</t>
+  </si>
+  <si>
+    <t>The Automation &lt;ProcessName&gt; encountered a system exception.</t>
+  </si>
+  <si>
+    <t>SystemException_EmailBody</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi Team,&lt;BR&gt;
+&lt;BR&gt;
+The automation for &lt;ProcessName&gt; encountered a system exception for the below reason(s):&lt;BR&gt;
+&lt;BR&gt;
+&lt;B&gt;Process Name:&lt;/B&gt; &lt;ProcessName&gt;&lt;BR&gt; 
+&lt;B&gt;Process Execution End Time:&lt;/B&gt; &lt;MM/DD/YYYY HH:MM AM/PM&gt;&lt;BR&gt; 
+&lt;B&gt;Process Status:&lt;/B&gt; &lt;SystemException&gt;&lt;BR&gt;
+&lt;BR&gt;
+&lt;B&gt;Execution Details:&lt;/B&gt; &lt;ProcessName&gt; has encountered a system exception due to &lt;SystemException&gt;. Please see the attached screenshot of the application issue the automation ran into. The Intelligent Automation Team is looking into this exception and will reach out shortly to you and review next steps.
+&lt;BR&gt;&lt;BR&gt;
+Thank you,&lt;BR&gt; 
+Intelligent Automation Team </t>
+  </si>
+  <si>
+    <t>BusinessException_EmailSubject</t>
+  </si>
+  <si>
+    <t>The Automation &lt;ProcessName&gt; encountered a business exception.</t>
+  </si>
+  <si>
+    <t>BusinessException_EmailBody</t>
+  </si>
+  <si>
+    <t>Hi Team,&lt;BR&gt;
+&lt;BR&gt;
+The automation for &lt;ProcessName&gt; encountered a business exception for the below reason(s):&lt;BR&gt;
+&lt;BR&gt;
+&lt;B&gt;Process Name:&lt;/B&gt; &lt;ProcessName&gt;&lt;BR&gt; 
+&lt;B&gt;Process Execution End Time:&lt;/B&gt; &lt;MM/DD/YYYY HH:MM AM/PM&gt;&lt;BR&gt; 
+&lt;B&gt;Process Status:&lt;/B&gt; &lt;BusinessException&gt;&lt;BR&gt;
+&lt;BR&gt;
+Please investigate this matter and process this transaction manually.&lt;BR&gt;
+&lt;BR&gt;&lt;BR&gt;
+Thank you,&lt;BR&gt; 
+Intelligent Automation Team</t>
+  </si>
+  <si>
+    <t>ExceptionEmail</t>
+  </si>
+  <si>
+    <t>BusinessExceptionEmail</t>
+  </si>
+  <si>
+    <t>EmailTemplatesFolderPath</t>
+  </si>
+  <si>
+    <t>HiringManagerTemplate_FileName</t>
+  </si>
+  <si>
+    <t>BOT_SharepointURL</t>
+  </si>
+  <si>
+    <t>P004_SP003_090_NewHireCommunication_WorkdayDisposition/Email Templates</t>
+  </si>
+  <si>
+    <t>Hiring Manager Template.xlsx</t>
+  </si>
+  <si>
+    <t>HMTemplateSheetName</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>WelcomeEmailTemplate_FileName</t>
+  </si>
+  <si>
+    <t>WETemplateSheetName</t>
+  </si>
+  <si>
+    <t>Welcome Email Template.xlsx</t>
+  </si>
+  <si>
+    <t>https://officemgmtentserv.sharepoint.com/sites/ACOE_Automations_DEV</t>
+  </si>
+  <si>
+    <t>Unable to login to Workday Application</t>
+  </si>
+  <si>
+    <t>Unable to find JR in Workday – &lt;JRNumber&gt;</t>
+  </si>
+  <si>
+    <t>Disposition not approved for more than 2 days- Needs Attention – “Employee Name”</t>
+  </si>
+  <si>
+    <t>Employee ID is in “Pre-Hire” in Workday after approval - Needs Attention – “Employee Name”</t>
+  </si>
+  <si>
+    <t>Unable to find Hiring Manager Template in shared location</t>
+  </si>
+  <si>
+    <t>System Exception_5</t>
+  </si>
+  <si>
+    <t>Unable to find Welcome Email Template in shared location</t>
+  </si>
+  <si>
+    <t>System Exception_1</t>
+  </si>
+  <si>
+    <t>Business Exception_1</t>
+  </si>
+  <si>
+    <t>Business Exception_2</t>
+  </si>
+  <si>
+    <t>Business Exception_3</t>
+  </si>
+  <si>
+    <t>Sytem Exception_2</t>
+  </si>
+  <si>
+    <t>System Exception_3</t>
+  </si>
+  <si>
+    <t>System Exception_4</t>
+  </si>
+  <si>
+    <t>Unable to download Hiring Manger Template from shared location</t>
+  </si>
+  <si>
+    <t>Unable to download  Welcome Email Template from shared location</t>
+  </si>
+  <si>
+    <t>System Exception_6</t>
+  </si>
+  <si>
+    <t>Invalid Calender Name</t>
+  </si>
+  <si>
+    <t>System Exception_7</t>
+  </si>
+  <si>
+    <t>System Exception_8</t>
+  </si>
+  <si>
+    <t>Maximum loop count reached to calculate working days</t>
+  </si>
+  <si>
+    <t>Unable to find working days in calender</t>
+  </si>
+  <si>
+    <t>CalenderLoopCount</t>
+  </si>
+  <si>
+    <t>CalenderName</t>
+  </si>
+  <si>
+    <t>NewHireComm_One</t>
+  </si>
+  <si>
+    <t>OrientationDay</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>RuntimeLocalFolderPath</t>
+  </si>
+  <si>
+    <t>C:\Users\&lt;Username&gt;\Documents\NHC Disposition Workday</t>
   </si>
 </sst>
 </file>
@@ -316,7 +476,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -330,6 +490,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -645,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z991"/>
+  <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -695,10 +858,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -709,7 +872,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -721,7 +884,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -732,44 +895,44 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
         <v>52</v>
@@ -777,97 +940,272 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
+        <v>58</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" t="s">
-        <v>54</v>
+        <v>59</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
         <v>62</v>
-      </c>
-      <c r="B14" s="5">
-        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" t="s">
-        <v>68</v>
+        <v>74</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+      <c r="A19" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A23" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A40" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A41" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A42" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A44" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -1811,10 +2149,11 @@
     <row r="989" ht="14.25" customHeight="1"/>
     <row r="990" ht="14.25" customHeight="1"/>
     <row r="991" ht="14.25" customHeight="1"/>
+    <row r="992" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1" xr:uid="{3C34412F-4442-4EA7-982D-69CB9A923319}"/>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{3C34412F-4442-4EA7-982D-69CB9A923319}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1825,7 +2164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -2009,7 +2348,7 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -2017,7 +2356,7 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -2025,7 +2364,7 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -2033,7 +2372,7 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B21">
         <v>15</v>
@@ -2041,7 +2380,7 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B22">
         <v>0.1</v>

</xml_diff>

<commit_message>
CR to include buliding name in welcome email
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56382C\Documents\UiPath\P004_SP003_090_NewHireCommunication_WorkdayDispositionApproval_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B811844-FC8F-4133-8F58-F2B55D235C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7D4494-1B1E-447A-8406-C19F565AF5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,27 @@
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Assets!$A$1:$D$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Assets!$A$1:$D$25</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="142">
   <si>
     <t>Name</t>
   </si>
@@ -170,9 +183,6 @@
     <t>O365ApplicationSecret</t>
   </si>
   <si>
-    <t>DEV</t>
-  </si>
-  <si>
     <t>P004_SP003_090_NHC_WD_ApprovalStat_Performer_Queue</t>
   </si>
   <si>
@@ -303,9 +313,6 @@
   </si>
   <si>
     <t>RuntimeLocalFolderPath</t>
-  </si>
-  <si>
-    <t>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</t>
   </si>
   <si>
     <t>P004_SP003_090_DispositionApproval_WaitDays</t>
@@ -472,19 +479,19 @@
     <t>P004_Shared_090_SharepointListName</t>
   </si>
   <si>
+    <t>P004_SP003_090_CalendarName</t>
+  </si>
+  <si>
+    <t>Shared_O365TenantID</t>
+  </si>
+  <si>
+    <t>Shared_O365ApplicationID</t>
+  </si>
+  <si>
+    <t>Shared_O365ApplicationSecret</t>
+  </si>
+  <si>
     <t>DEV/P004_NewHireCommunication</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_O365AppID</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_O365TenantID</t>
-  </si>
-  <si>
-    <t>P004_Shared_090_O365ApplicationSecret</t>
-  </si>
-  <si>
-    <t>P004_SP003_090_CalendarName</t>
   </si>
 </sst>
 </file>
@@ -568,9 +575,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -608,7 +615,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -714,7 +721,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -856,7 +863,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -866,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z970"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -914,10 +921,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -928,7 +935,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>141</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -940,7 +947,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -948,119 +955,119 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" t="s">
         <v>82</v>
-      </c>
-      <c r="B15" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -1068,39 +1075,61 @@
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
+        <v>101</v>
+      </c>
+      <c r="B21" t="str">
+        <f>B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>140</v>
+      </c>
+    </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2239,7 +2268,7 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -2247,7 +2276,7 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -2255,7 +2284,7 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -2263,7 +2292,7 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21">
         <v>15</v>
@@ -2271,7 +2300,7 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22">
         <v>0.1</v>
@@ -2279,7 +2308,7 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -3257,10 +3286,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3312,10 +3341,11 @@
         <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>139</v>
+        <v>125</v>
+      </c>
+      <c r="C2" s="2" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3323,287 +3353,280 @@
         <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>139</v>
+        <v>126</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>139</v>
+        <v>128</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>139</v>
+      <c r="C7" s="2" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>139</v>
+        <v>130</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>139</v>
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>139</v>
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>139</v>
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" t="s">
-        <v>92</v>
+        <v>54</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
         <v>94</v>
       </c>
-      <c r="C13" t="s">
-        <v>92</v>
+      <c r="C13" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
         <v>95</v>
       </c>
-      <c r="C14" t="s">
-        <v>92</v>
+      <c r="C14" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>139</v>
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" t="s">
-        <v>92</v>
+        <v>97</v>
+      </c>
+      <c r="C16" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" t="s">
-        <v>92</v>
+        <v>98</v>
+      </c>
+      <c r="C17" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" t="s">
-        <v>92</v>
+        <v>68</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="2" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" t="s">
-        <v>92</v>
+        <v>137</v>
+      </c>
+      <c r="C19" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" t="s">
-        <v>92</v>
+        <v>99</v>
+      </c>
+      <c r="C20" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>139</v>
+        <v>104</v>
+      </c>
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s">
-        <v>143</v>
-      </c>
-      <c r="C22" t="s">
-        <v>92</v>
+        <v>110</v>
+      </c>
+      <c r="C22" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>DEV/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" t="s">
-        <v>92</v>
+        <v>113</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="2" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" t="s">
-        <v>105</v>
-      </c>
-      <c r="C24" t="s">
-        <v>92</v>
+        <v>116</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="2" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" t="s">
-        <v>115</v>
-      </c>
-      <c r="B26" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
-        <v>119</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
+      <c r="C25" s="2" t="str">
+        <f>Settings!B3</f>
+        <v>DEV/P004_NewHireCommunication</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4572,11 +4595,11 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C12 C18" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added change to pick workday employee name
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56382C\Documents\UiPath\P004_SP003_090_NewHireCommunication_WorkdayDispositionApproval_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F2E220-54B1-4C6E-BB7D-70B26B871F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273870B4-4531-4B92-BBF1-18F393428A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="145">
   <si>
     <t>Name</t>
   </si>
@@ -489,6 +489,15 @@
   </si>
   <si>
     <t>Shared_O365ApplicationSecret</t>
+  </si>
+  <si>
+    <t>BOTCredentialAssetName</t>
+  </si>
+  <si>
+    <t>P004_SP003_090_BOT_Credentials</t>
+  </si>
+  <si>
+    <t>ProcessAssetFolderPath</t>
   </si>
   <si>
     <t>PROD/P004_NewHireCommunication</t>
@@ -575,9 +584,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -615,7 +624,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -721,7 +730,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -863,7 +872,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -873,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z970"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -935,7 +944,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -1130,8 +1139,23 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>143</v>
+      </c>
+      <c r="B29" t="str">
+        <f>Settings!B3&amp;"/SP_003_WorkdayDisposition"</f>
+        <v>PROD/P004_NewHireCommunication/SP_003_WorkdayDisposition</v>
+      </c>
+    </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2084,7 +2108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -3289,7 +3313,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>